<commit_message>
fixed fg wb yml files
</commit_message>
<xml_diff>
--- a/Mordheim-BorderTownBurning/Warband Rosters/kai/forest_goblins/forest_goblins_20.xlsx
+++ b/Mordheim-BorderTownBurning/Warband Rosters/kai/forest_goblins/forest_goblins_20.xlsx
@@ -1010,7 +1010,7 @@
   <dimension ref="B2:Q44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1045,14 +1045,14 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="3" t="n">
-        <v>43650</v>
+        <v>43651</v>
       </c>
       <c r="I2" s="0" t="s">
         <v>2</v>
       </c>
       <c r="J2" s="4" t="n">
         <f aca="false">J3+(3*'Hired swords'!B5)+H38+I38+J38</f>
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1066,7 +1066,7 @@
       </c>
       <c r="J3" s="7" t="n">
         <f aca="false">E18+'Hired swords'!B19</f>
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="J4" s="8" t="n">
         <f aca="false">'Characteristic analysis'!J29+'Hired swords'!O19</f>
-        <v>1331</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1099,14 +1099,14 @@
       </c>
       <c r="C6" s="9" t="n">
         <f aca="false">G18+N42+'Hired swords'!G19</f>
-        <v>491</v>
+        <v>474</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J6" s="9" t="n">
         <f aca="false">5*(E18-E17)+E11*F11+E12*F12+E13*F13+E14*F14+E15*F15+E16*F16+E17*20+SUM(H38:J38)*10+'Hired swords'!I19</f>
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1115,7 +1115,7 @@
       </c>
       <c r="C7" s="11" t="n">
         <f aca="false">C5-C6</f>
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>11</v>
@@ -1138,11 +1138,11 @@
       </c>
       <c r="J8" s="13" t="n">
         <f aca="false">Q42</f>
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K8" s="0" t="n">
         <f aca="false">Q43</f>
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L8" s="0" t="n">
         <f aca="false">Q44</f>
@@ -1152,7 +1152,7 @@
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J9" s="7" t="n">
         <f aca="false">(J4+J5+J6+J8)*J7</f>
-        <v>7585</v>
+        <v>7225</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1245,13 +1245,13 @@
       </c>
       <c r="I13" s="0" t="n">
         <f aca="false">J6+J6*50%</f>
-        <v>184.5</v>
+        <v>177</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K13" s="0" t="n">
-        <v>288</v>
+        <v>192</v>
       </c>
       <c r="N13" s="0" t="s">
         <v>28</v>
@@ -1271,18 +1271,18 @@
         <v>15</v>
       </c>
       <c r="E14" s="16" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F14" s="16" t="n">
         <v>0</v>
       </c>
       <c r="G14" s="0" t="n">
         <f aca="false">E14*D14</f>
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="I14" s="1" t="n">
         <f aca="false">J6+J6*75%</f>
-        <v>215.25</v>
+        <v>206.5</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>32</v>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="I15" s="1" t="n">
         <f aca="false">J6+J6*100%</f>
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>35</v>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="I16" s="1" t="n">
         <f aca="false">J6+J6*150%</f>
-        <v>307.5</v>
+        <v>295</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>39</v>
@@ -1372,7 +1372,7 @@
       </c>
       <c r="I17" s="0" t="n">
         <f aca="false">J6+J6*300%</f>
-        <v>492</v>
+        <v>472</v>
       </c>
       <c r="J17" s="20" t="s">
         <v>41</v>
@@ -1384,11 +1384,11 @@
       </c>
       <c r="E18" s="7" t="n">
         <f aca="false">SUM(E11:E17)+C44</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G18" s="7" t="n">
         <f aca="false">SUM(G11:G17)</f>
-        <v>340</v>
+        <v>325</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1503,7 +1503,7 @@
       </c>
       <c r="K22" s="0" t="n">
         <f aca="false">E14</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L22" s="0" t="n">
         <f aca="false">E15</f>
@@ -1525,7 +1525,7 @@
       </c>
       <c r="Q22" s="1" t="n">
         <f aca="false">P22*SUM(H22:M22)</f>
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1555,7 +1555,7 @@
       </c>
       <c r="K23" s="0" t="n">
         <f aca="false">E14</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L23" s="0" t="n">
         <v>0</v>
@@ -1565,7 +1565,7 @@
       </c>
       <c r="N23" s="0" t="n">
         <f aca="false">SUM(H23:M23)*G23</f>
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>59</v>
@@ -1575,7 +1575,7 @@
       </c>
       <c r="Q23" s="1" t="n">
         <f aca="false">P23*SUM(H23:M23)</f>
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2425,7 +2425,7 @@
       </c>
       <c r="K42" s="27" t="n">
         <f aca="false">K22*$G22+K23*$G23+K24*$G24+K25*$G25+K26*$G26+K27*$G27+K28*$G28+K29*$G29+K30*$G30+K31*$G31+K32*$G32+K33*$G33+K34*$G34+K35*$G35+K36*$G36+K37*$G37+K38*$G38+K39*$G39+G40*K40</f>
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L42" s="27" t="n">
         <f aca="false">L22*$G22+L23*$G23+L24*$G24+L25*$G25+L26*$G26+L27*$G27+L28*$G28+L29*$G29+L30*$G30+L31*$G31+L32*$G32+L33*$G33+L34*$G34+L35*$G35+L36*$G36+L37*$G37+L38*$G38+L39*$G39+G40*L40</f>
@@ -2437,7 +2437,7 @@
       </c>
       <c r="N42" s="7" t="n">
         <f aca="false">SUM(N22:N40)</f>
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="O42" s="22"/>
       <c r="P42" s="0" t="s">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="Q42" s="7" t="n">
         <f aca="false">SUM(Q22:Q40)</f>
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2461,7 +2461,7 @@
       </c>
       <c r="Q43" s="0" t="n">
         <f aca="false">SUM(Q22:Q40)-Q44</f>
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2578,101 +2578,101 @@
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="n">
         <f aca="false">'cost calculation'!K13</f>
-        <v>288</v>
+        <v>192</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">C3+15</f>
-        <v>303</v>
+        <v>207</v>
       </c>
       <c r="E3" s="0" t="n">
         <f aca="false">D3+15</f>
-        <v>318</v>
+        <v>222</v>
       </c>
       <c r="F3" s="0" t="n">
         <f aca="false">E3+15</f>
-        <v>333</v>
+        <v>237</v>
       </c>
       <c r="G3" s="0" t="n">
         <f aca="false">F3+15</f>
-        <v>348</v>
+        <v>252</v>
       </c>
       <c r="H3" s="0" t="n">
         <f aca="false">G3+15</f>
-        <v>363</v>
+        <v>267</v>
       </c>
       <c r="I3" s="0" t="n">
         <f aca="false">H3+15</f>
-        <v>378</v>
+        <v>282</v>
       </c>
       <c r="J3" s="0" t="n">
         <f aca="false">I3+15</f>
-        <v>393</v>
+        <v>297</v>
       </c>
       <c r="K3" s="0" t="n">
         <f aca="false">J3+15</f>
-        <v>408</v>
+        <v>312</v>
       </c>
       <c r="L3" s="0" t="n">
         <f aca="false">K3+15</f>
-        <v>423</v>
+        <v>327</v>
       </c>
       <c r="M3" s="0" t="n">
         <f aca="false">L3+15</f>
-        <v>438</v>
+        <v>342</v>
       </c>
       <c r="N3" s="0" t="n">
         <f aca="false">M3+15</f>
-        <v>453</v>
+        <v>357</v>
       </c>
       <c r="O3" s="0" t="n">
         <f aca="false">N3+15</f>
-        <v>468</v>
+        <v>372</v>
       </c>
       <c r="P3" s="0" t="n">
         <f aca="false">O3+15</f>
-        <v>483</v>
+        <v>387</v>
       </c>
       <c r="Q3" s="0" t="n">
         <f aca="false">P3+15</f>
-        <v>498</v>
+        <v>402</v>
       </c>
       <c r="R3" s="0" t="n">
         <f aca="false">Q3+15</f>
-        <v>513</v>
+        <v>417</v>
       </c>
       <c r="S3" s="0" t="n">
         <f aca="false">R3+15</f>
-        <v>528</v>
+        <v>432</v>
       </c>
       <c r="T3" s="0" t="n">
         <f aca="false">S3+15</f>
-        <v>543</v>
+        <v>447</v>
       </c>
       <c r="U3" s="0" t="n">
         <f aca="false">T3+15</f>
-        <v>558</v>
+        <v>462</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="28" t="n">
         <f aca="false">IF(B10&lt;C3,$A10,IF(B9&lt;C3,$A9,IF(B8&lt;C3,$A8,IF(B7&lt;C3,$A7,IF(B6&lt;C3,$A6,1)))))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4" s="28" t="n">
         <f aca="false">IF(C10&lt;D3,$A10,IF(C9&lt;D3,$A9,IF(C8&lt;D3,$A8,IF(C7&lt;D3,$A7,IF(C6&lt;D3,$A6,1)))))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E4" s="28" t="n">
         <f aca="false">IF(D10&lt;E3,$A10,IF(D9&lt;E3,$A9,IF(D8&lt;E3,$A8,IF(D7&lt;E3,$A7,IF(D6&lt;E3,$A6,1)))))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F4" s="28" t="n">
         <f aca="false">IF(E10&lt;F3,$A10,IF(E9&lt;F3,$A9,IF(E8&lt;F3,$A8,IF(E7&lt;F3,$A7,IF(E6&lt;F3,$A6,1)))))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G4" s="28" t="n">
         <f aca="false">IF(F10&lt;G3,$A10,IF(F9&lt;G3,$A9,IF(F8&lt;G3,$A8,IF(F7&lt;G3,$A7,IF(F6&lt;G3,$A6,1)))))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H4" s="28" t="n">
         <f aca="false">IF(G10&lt;H3,$A10,IF(G9&lt;H3,$A9,IF(G8&lt;H3,$A8,IF(G7&lt;H3,$A7,IF(G6&lt;H3,$A6,1)))))</f>
@@ -2692,7 +2692,7 @@
       </c>
       <c r="L4" s="28" t="n">
         <f aca="false">IF(K10&lt;L3,$A10,IF(K9&lt;L3,$A9,IF(K8&lt;L3,$A8,IF(K7&lt;L3,$A7,IF(K6&lt;L3,$A6,1)))))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M4" s="28" t="n">
         <f aca="false">IF(L10&lt;M3,$A10,IF(L9&lt;M3,$A9,IF(L8&lt;M3,$A8,IF(L7&lt;M3,$A7,IF(L6&lt;M3,$A6,1)))))</f>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="S4" s="28" t="n">
         <f aca="false">IF(R10&lt;S3,$A10,IF(R9&lt;S3,$A9,IF(R8&lt;S3,$A8,IF(R7&lt;S3,$A7,IF(R6&lt;S3,$A6,1)))))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T4" s="28" t="n">
         <f aca="false">IF(S10&lt;T3,$A10,IF(S9&lt;T3,$A9,IF(S8&lt;T3,$A8,IF(S7&lt;T3,$A7,IF(S6&lt;T3,$A6,1)))))</f>
@@ -2734,83 +2734,83 @@
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="n">
         <f aca="false">'cost calculation'!J6</f>
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C5" s="0" t="n">
         <f aca="false">B5+3*C4</f>
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">C5+3*D4</f>
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="E5" s="0" t="n">
         <f aca="false">D5+3*E4</f>
-        <v>159</v>
+        <v>136</v>
       </c>
       <c r="F5" s="0" t="n">
         <f aca="false">E5+3*F4</f>
-        <v>171</v>
+        <v>142</v>
       </c>
       <c r="G5" s="0" t="n">
         <f aca="false">F5+3*G4</f>
-        <v>183</v>
+        <v>151</v>
       </c>
       <c r="H5" s="0" t="n">
         <f aca="false">G5+3*H4</f>
-        <v>192</v>
+        <v>160</v>
       </c>
       <c r="I5" s="0" t="n">
         <f aca="false">H5+3*I4</f>
-        <v>201</v>
+        <v>169</v>
       </c>
       <c r="J5" s="0" t="n">
         <f aca="false">I5+3*J4</f>
-        <v>210</v>
+        <v>178</v>
       </c>
       <c r="K5" s="0" t="n">
         <f aca="false">J5+3*K4</f>
-        <v>219</v>
+        <v>187</v>
       </c>
       <c r="L5" s="0" t="n">
         <f aca="false">K5+3*L4</f>
-        <v>228</v>
+        <v>193</v>
       </c>
       <c r="M5" s="0" t="n">
         <f aca="false">L5+3*M4</f>
-        <v>237</v>
+        <v>202</v>
       </c>
       <c r="N5" s="0" t="n">
         <f aca="false">M5+3*N4</f>
-        <v>246</v>
+        <v>211</v>
       </c>
       <c r="O5" s="0" t="n">
         <f aca="false">N5+3*O4</f>
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="P5" s="0" t="n">
         <f aca="false">O5+3*P4</f>
-        <v>264</v>
+        <v>229</v>
       </c>
       <c r="Q5" s="0" t="n">
         <f aca="false">P5+3*Q4</f>
-        <v>273</v>
+        <v>238</v>
       </c>
       <c r="R5" s="0" t="n">
         <f aca="false">Q5+3*R4</f>
-        <v>282</v>
+        <v>247</v>
       </c>
       <c r="S5" s="0" t="n">
         <f aca="false">R5+3*S4</f>
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="T5" s="0" t="n">
         <f aca="false">S5+3*T4</f>
-        <v>300</v>
+        <v>262</v>
       </c>
       <c r="U5" s="0" t="n">
         <f aca="false">T5+3*U4</f>
-        <v>309</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2819,83 +2819,83 @@
       </c>
       <c r="B6" s="0" t="n">
         <f aca="false">B$5+B$5*50%</f>
-        <v>184.5</v>
+        <v>177</v>
       </c>
       <c r="C6" s="0" t="n">
         <f aca="false">C$5+C$5*50%</f>
-        <v>202.5</v>
+        <v>186</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">D$5+D$5*50%</f>
-        <v>220.5</v>
+        <v>195</v>
       </c>
       <c r="E6" s="0" t="n">
         <f aca="false">E$5+E$5*50%</f>
-        <v>238.5</v>
+        <v>204</v>
       </c>
       <c r="F6" s="0" t="n">
         <f aca="false">F$5+F$5*50%</f>
-        <v>256.5</v>
+        <v>213</v>
       </c>
       <c r="G6" s="0" t="n">
         <f aca="false">G$5+G$5*50%</f>
-        <v>274.5</v>
+        <v>226.5</v>
       </c>
       <c r="H6" s="0" t="n">
         <f aca="false">H$5+H$5*50%</f>
-        <v>288</v>
+        <v>240</v>
       </c>
       <c r="I6" s="0" t="n">
         <f aca="false">I$5+I$5*50%</f>
-        <v>301.5</v>
+        <v>253.5</v>
       </c>
       <c r="J6" s="0" t="n">
         <f aca="false">J$5+J$5*50%</f>
-        <v>315</v>
+        <v>267</v>
       </c>
       <c r="K6" s="0" t="n">
         <f aca="false">K$5+K$5*50%</f>
-        <v>328.5</v>
+        <v>280.5</v>
       </c>
       <c r="L6" s="0" t="n">
         <f aca="false">L$5+L$5*50%</f>
-        <v>342</v>
+        <v>289.5</v>
       </c>
       <c r="M6" s="0" t="n">
         <f aca="false">M$5+M$5*50%</f>
-        <v>355.5</v>
+        <v>303</v>
       </c>
       <c r="N6" s="0" t="n">
         <f aca="false">N$5+N$5*50%</f>
-        <v>369</v>
+        <v>316.5</v>
       </c>
       <c r="O6" s="0" t="n">
         <f aca="false">O$5+O$5*50%</f>
-        <v>382.5</v>
+        <v>330</v>
       </c>
       <c r="P6" s="0" t="n">
         <f aca="false">P$5+P$5*50%</f>
-        <v>396</v>
+        <v>343.5</v>
       </c>
       <c r="Q6" s="0" t="n">
         <f aca="false">Q$5+Q$5*50%</f>
-        <v>409.5</v>
+        <v>357</v>
       </c>
       <c r="R6" s="0" t="n">
         <f aca="false">R$5+R$5*50%</f>
-        <v>423</v>
+        <v>370.5</v>
       </c>
       <c r="S6" s="0" t="n">
         <f aca="false">S$5+S$5*50%</f>
-        <v>436.5</v>
+        <v>379.5</v>
       </c>
       <c r="T6" s="0" t="n">
         <f aca="false">T$5+T$5*50%</f>
-        <v>450</v>
+        <v>393</v>
       </c>
       <c r="U6" s="0" t="n">
         <f aca="false">U$5+U$5*50%</f>
-        <v>463.5</v>
+        <v>406.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2904,83 +2904,83 @@
       </c>
       <c r="B7" s="0" t="n">
         <f aca="false">B$5+B$5*75%</f>
-        <v>215.25</v>
+        <v>206.5</v>
       </c>
       <c r="C7" s="0" t="n">
         <f aca="false">C$5+C$5*75%</f>
-        <v>236.25</v>
+        <v>217</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">D$5+D$5*75%</f>
-        <v>257.25</v>
+        <v>227.5</v>
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">E$5+E$5*75%</f>
-        <v>278.25</v>
+        <v>238</v>
       </c>
       <c r="F7" s="0" t="n">
         <f aca="false">F$5+F$5*75%</f>
-        <v>299.25</v>
+        <v>248.5</v>
       </c>
       <c r="G7" s="0" t="n">
         <f aca="false">G$5+G$5*75%</f>
-        <v>320.25</v>
+        <v>264.25</v>
       </c>
       <c r="H7" s="0" t="n">
         <f aca="false">H$5+H$5*75%</f>
-        <v>336</v>
+        <v>280</v>
       </c>
       <c r="I7" s="0" t="n">
         <f aca="false">I$5+I$5*75%</f>
-        <v>351.75</v>
+        <v>295.75</v>
       </c>
       <c r="J7" s="0" t="n">
         <f aca="false">J$5+J$5*75%</f>
-        <v>367.5</v>
+        <v>311.5</v>
       </c>
       <c r="K7" s="0" t="n">
         <f aca="false">K$5+K$5*75%</f>
-        <v>383.25</v>
+        <v>327.25</v>
       </c>
       <c r="L7" s="0" t="n">
         <f aca="false">L$5+L$5*75%</f>
-        <v>399</v>
+        <v>337.75</v>
       </c>
       <c r="M7" s="0" t="n">
         <f aca="false">M$5+M$5*75%</f>
-        <v>414.75</v>
+        <v>353.5</v>
       </c>
       <c r="N7" s="0" t="n">
         <f aca="false">N$5+N$5*75%</f>
-        <v>430.5</v>
+        <v>369.25</v>
       </c>
       <c r="O7" s="0" t="n">
         <f aca="false">O$5+O$5*75%</f>
-        <v>446.25</v>
+        <v>385</v>
       </c>
       <c r="P7" s="0" t="n">
         <f aca="false">P$5+P$5*75%</f>
-        <v>462</v>
+        <v>400.75</v>
       </c>
       <c r="Q7" s="0" t="n">
         <f aca="false">Q$5+Q$5*75%</f>
-        <v>477.75</v>
+        <v>416.5</v>
       </c>
       <c r="R7" s="0" t="n">
         <f aca="false">R$5+R$5*75%</f>
-        <v>493.5</v>
+        <v>432.25</v>
       </c>
       <c r="S7" s="0" t="n">
         <f aca="false">S$5+S$5*75%</f>
-        <v>509.25</v>
+        <v>442.75</v>
       </c>
       <c r="T7" s="0" t="n">
         <f aca="false">T$5+T$5*75%</f>
-        <v>525</v>
+        <v>458.5</v>
       </c>
       <c r="U7" s="0" t="n">
         <f aca="false">U$5+U$5*75%</f>
-        <v>540.75</v>
+        <v>474.25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2989,83 +2989,83 @@
       </c>
       <c r="B8" s="0" t="n">
         <f aca="false">B$5+B$5*100%</f>
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C8" s="0" t="n">
         <f aca="false">C$5+C$5*100%</f>
-        <v>270</v>
+        <v>248</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">D$5+D$5*100%</f>
-        <v>294</v>
+        <v>260</v>
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">E$5+E$5*100%</f>
-        <v>318</v>
+        <v>272</v>
       </c>
       <c r="F8" s="0" t="n">
         <f aca="false">F$5+F$5*100%</f>
-        <v>342</v>
+        <v>284</v>
       </c>
       <c r="G8" s="0" t="n">
         <f aca="false">G$5+G$5*100%</f>
-        <v>366</v>
+        <v>302</v>
       </c>
       <c r="H8" s="0" t="n">
         <f aca="false">H$5+H$5*100%</f>
-        <v>384</v>
+        <v>320</v>
       </c>
       <c r="I8" s="0" t="n">
         <f aca="false">I$5+I$5*100%</f>
-        <v>402</v>
+        <v>338</v>
       </c>
       <c r="J8" s="0" t="n">
         <f aca="false">J$5+J$5*100%</f>
-        <v>420</v>
+        <v>356</v>
       </c>
       <c r="K8" s="0" t="n">
         <f aca="false">K$5+K$5*100%</f>
-        <v>438</v>
+        <v>374</v>
       </c>
       <c r="L8" s="0" t="n">
         <f aca="false">L$5+L$5*100%</f>
-        <v>456</v>
+        <v>386</v>
       </c>
       <c r="M8" s="0" t="n">
         <f aca="false">M$5+M$5*100%</f>
-        <v>474</v>
+        <v>404</v>
       </c>
       <c r="N8" s="0" t="n">
         <f aca="false">N$5+N$5*100%</f>
-        <v>492</v>
+        <v>422</v>
       </c>
       <c r="O8" s="0" t="n">
         <f aca="false">O$5+O$5*100%</f>
-        <v>510</v>
+        <v>440</v>
       </c>
       <c r="P8" s="0" t="n">
         <f aca="false">P$5+P$5*100%</f>
-        <v>528</v>
+        <v>458</v>
       </c>
       <c r="Q8" s="0" t="n">
         <f aca="false">Q$5+Q$5*100%</f>
-        <v>546</v>
+        <v>476</v>
       </c>
       <c r="R8" s="0" t="n">
         <f aca="false">R$5+R$5*100%</f>
-        <v>564</v>
+        <v>494</v>
       </c>
       <c r="S8" s="0" t="n">
         <f aca="false">S$5+S$5*100%</f>
-        <v>582</v>
+        <v>506</v>
       </c>
       <c r="T8" s="0" t="n">
         <f aca="false">T$5+T$5*100%</f>
-        <v>600</v>
+        <v>524</v>
       </c>
       <c r="U8" s="0" t="n">
         <f aca="false">U$5+U$5*100%</f>
-        <v>618</v>
+        <v>542</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3074,83 +3074,83 @@
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">B$5+B$5*150%</f>
-        <v>307.5</v>
+        <v>295</v>
       </c>
       <c r="C9" s="0" t="n">
         <f aca="false">C$5+C$5*150%</f>
-        <v>337.5</v>
+        <v>310</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">D$5+D$5*150%</f>
-        <v>367.5</v>
+        <v>325</v>
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">E$5+E$5*150%</f>
-        <v>397.5</v>
+        <v>340</v>
       </c>
       <c r="F9" s="0" t="n">
         <f aca="false">F$5+F$5*150%</f>
-        <v>427.5</v>
+        <v>355</v>
       </c>
       <c r="G9" s="0" t="n">
         <f aca="false">G$5+G$5*150%</f>
-        <v>457.5</v>
+        <v>377.5</v>
       </c>
       <c r="H9" s="0" t="n">
         <f aca="false">H$5+H$5*150%</f>
-        <v>480</v>
+        <v>400</v>
       </c>
       <c r="I9" s="0" t="n">
         <f aca="false">I$5+I$5*150%</f>
-        <v>502.5</v>
+        <v>422.5</v>
       </c>
       <c r="J9" s="0" t="n">
         <f aca="false">J$5+J$5*150%</f>
-        <v>525</v>
+        <v>445</v>
       </c>
       <c r="K9" s="0" t="n">
         <f aca="false">K$5+K$5*150%</f>
-        <v>547.5</v>
+        <v>467.5</v>
       </c>
       <c r="L9" s="0" t="n">
         <f aca="false">L$5+L$5*150%</f>
-        <v>570</v>
+        <v>482.5</v>
       </c>
       <c r="M9" s="0" t="n">
         <f aca="false">M$5+M$5*150%</f>
-        <v>592.5</v>
+        <v>505</v>
       </c>
       <c r="N9" s="0" t="n">
         <f aca="false">N$5+N$5*150%</f>
-        <v>615</v>
+        <v>527.5</v>
       </c>
       <c r="O9" s="0" t="n">
         <f aca="false">O$5+O$5*150%</f>
-        <v>637.5</v>
+        <v>550</v>
       </c>
       <c r="P9" s="0" t="n">
         <f aca="false">P$5+P$5*150%</f>
-        <v>660</v>
+        <v>572.5</v>
       </c>
       <c r="Q9" s="0" t="n">
         <f aca="false">Q$5+Q$5*150%</f>
-        <v>682.5</v>
+        <v>595</v>
       </c>
       <c r="R9" s="0" t="n">
         <f aca="false">R$5+R$5*150%</f>
-        <v>705</v>
+        <v>617.5</v>
       </c>
       <c r="S9" s="0" t="n">
         <f aca="false">S$5+S$5*150%</f>
-        <v>727.5</v>
+        <v>632.5</v>
       </c>
       <c r="T9" s="0" t="n">
         <f aca="false">T$5+T$5*150%</f>
-        <v>750</v>
+        <v>655</v>
       </c>
       <c r="U9" s="0" t="n">
         <f aca="false">U$5+U$5*150%</f>
-        <v>772.5</v>
+        <v>677.5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3159,161 +3159,161 @@
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">B$5+B$5*300%</f>
-        <v>492</v>
+        <v>472</v>
       </c>
       <c r="C10" s="0" t="n">
         <f aca="false">C$5+C$5*300%</f>
-        <v>540</v>
+        <v>496</v>
       </c>
       <c r="D10" s="0" t="n">
         <f aca="false">D$5+D$5*300%</f>
-        <v>588</v>
+        <v>520</v>
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">E$5+E$5*300%</f>
-        <v>636</v>
+        <v>544</v>
       </c>
       <c r="F10" s="0" t="n">
         <f aca="false">F$5+F$5*300%</f>
-        <v>684</v>
+        <v>568</v>
       </c>
       <c r="G10" s="0" t="n">
         <f aca="false">G$5+G$5*300%</f>
-        <v>732</v>
+        <v>604</v>
       </c>
       <c r="H10" s="0" t="n">
         <f aca="false">H$5+H$5*300%</f>
-        <v>768</v>
+        <v>640</v>
       </c>
       <c r="I10" s="0" t="n">
         <f aca="false">I$5+I$5*300%</f>
-        <v>804</v>
+        <v>676</v>
       </c>
       <c r="J10" s="0" t="n">
         <f aca="false">J$5+J$5*300%</f>
-        <v>840</v>
+        <v>712</v>
       </c>
       <c r="K10" s="0" t="n">
         <f aca="false">K$5+K$5*300%</f>
-        <v>876</v>
+        <v>748</v>
       </c>
       <c r="L10" s="0" t="n">
         <f aca="false">L$5+L$5*300%</f>
-        <v>912</v>
+        <v>772</v>
       </c>
       <c r="M10" s="0" t="n">
         <f aca="false">M$5+M$5*300%</f>
-        <v>948</v>
+        <v>808</v>
       </c>
       <c r="N10" s="0" t="n">
         <f aca="false">N$5+N$5*300%</f>
-        <v>984</v>
+        <v>844</v>
       </c>
       <c r="O10" s="0" t="n">
         <f aca="false">O$5+O$5*300%</f>
-        <v>1020</v>
+        <v>880</v>
       </c>
       <c r="P10" s="0" t="n">
         <f aca="false">P$5+P$5*300%</f>
-        <v>1056</v>
+        <v>916</v>
       </c>
       <c r="Q10" s="0" t="n">
         <f aca="false">Q$5+Q$5*300%</f>
-        <v>1092</v>
+        <v>952</v>
       </c>
       <c r="R10" s="0" t="n">
         <f aca="false">R$5+R$5*300%</f>
-        <v>1128</v>
+        <v>988</v>
       </c>
       <c r="S10" s="0" t="n">
         <f aca="false">S$5+S$5*300%</f>
-        <v>1164</v>
+        <v>1012</v>
       </c>
       <c r="T10" s="0" t="n">
         <f aca="false">T$5+T$5*300%</f>
-        <v>1200</v>
+        <v>1048</v>
       </c>
       <c r="U10" s="0" t="n">
         <f aca="false">U$5+U$5*300%</f>
-        <v>1236</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="28" t="n">
         <f aca="false">C4*('cost calculation'!$J$3-'cost calculation'!$E$17)</f>
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="D11" s="28" t="n">
         <f aca="false">D4*('cost calculation'!$J$3-'cost calculation'!$E$17)</f>
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="E11" s="28" t="n">
         <f aca="false">E4*('cost calculation'!$J$3-'cost calculation'!$E$17)</f>
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="F11" s="28" t="n">
         <f aca="false">F4*('cost calculation'!$J$3-'cost calculation'!$E$17)</f>
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="G11" s="28" t="n">
         <f aca="false">G4*('cost calculation'!$J$3-'cost calculation'!$E$17)</f>
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="H11" s="28" t="n">
         <f aca="false">H4*('cost calculation'!$J$3-'cost calculation'!$E$17)</f>
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I11" s="28" t="n">
         <f aca="false">I4*('cost calculation'!$J$3-'cost calculation'!$E$17)</f>
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J11" s="28" t="n">
         <f aca="false">J4*('cost calculation'!$J$3-'cost calculation'!$E$17)</f>
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K11" s="28" t="n">
         <f aca="false">K4*('cost calculation'!$J$3-'cost calculation'!$E$17)</f>
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L11" s="28" t="n">
         <f aca="false">L4*('cost calculation'!$J$3-'cost calculation'!$E$17)</f>
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="M11" s="28" t="n">
         <f aca="false">M4*('cost calculation'!$J$3-'cost calculation'!$E$17)</f>
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N11" s="28" t="n">
         <f aca="false">N4*('cost calculation'!$J$3-'cost calculation'!$E$17)</f>
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="O11" s="28" t="n">
         <f aca="false">O4*('cost calculation'!$J$3-'cost calculation'!$E$17)</f>
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="P11" s="28" t="n">
         <f aca="false">P4*('cost calculation'!$J$3-'cost calculation'!$E$17)</f>
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q11" s="28" t="n">
         <f aca="false">Q4*('cost calculation'!$J$3-'cost calculation'!$E$17)</f>
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="R11" s="28" t="n">
         <f aca="false">R4*('cost calculation'!$J$3-'cost calculation'!$E$17)</f>
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="S11" s="28" t="n">
         <f aca="false">S4*('cost calculation'!$J$3-'cost calculation'!$E$17)</f>
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="T11" s="28" t="n">
         <f aca="false">T4*('cost calculation'!$J$3-'cost calculation'!$E$17)</f>
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="U11" s="28" t="n">
         <f aca="false">U4*('cost calculation'!$J$3-'cost calculation'!$E$17)</f>
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -3335,7 +3335,7 @@
   <dimension ref="B2:O19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4211,10 +4211,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:L29"/>
+  <dimension ref="B2:L31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="M31" activeCellId="0" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4963,7 +4963,7 @@
       </c>
       <c r="F28" s="31" t="n">
         <f aca="false">'cost calculation'!$E14*'Characteristic analysis'!F27</f>
-        <v>77.9999999999999</v>
+        <v>73.6666666666666</v>
       </c>
       <c r="G28" s="31" t="n">
         <f aca="false">'cost calculation'!$E15*'Characteristic analysis'!G27</f>
@@ -4979,7 +4979,7 @@
       </c>
       <c r="J28" s="8" t="n">
         <f aca="false">SUM(C28:I28)</f>
-        <v>84.2799999999999</v>
+        <v>79.9466666666666</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4997,7 +4997,7 @@
       </c>
       <c r="F29" s="31" t="n">
         <f aca="false">'cost calculation'!$E14*(F5*$L5+F6*$L6+F7*$L7+F8*$L8+F9*$L9+F10*$L10+F11*$L11+F12*$L12+F13*$L13)</f>
-        <v>1170</v>
+        <v>1105</v>
       </c>
       <c r="G29" s="31" t="n">
         <f aca="false">'cost calculation'!$E15*(G5*$L5+G6*$L6+G7*$L7+G8*$L8+G9*$L9+G10*$L10+G11*$L11+G12*$L12+G13*$L13)</f>
@@ -5013,9 +5013,10 @@
       </c>
       <c r="J29" s="8" t="n">
         <f aca="false">SUM(C29:I29)</f>
-        <v>1331</v>
-      </c>
-    </row>
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C3:F3"/>

</xml_diff>